<commit_message>
Aula 11 - Herança e Exceções ==> Falta alguns exercicios
</commit_message>
<xml_diff>
--- a/GRANDE_PORTE/Java MF - BRQ - SET22/Arquitetura/Atalhos-Plugins-Intellij.xlsx
+++ b/GRANDE_PORTE/Java MF - BRQ - SET22/Arquitetura/Atalhos-Plugins-Intellij.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{02FAB793-CB38-4888-8DA9-CA2DD851CDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C05C1D-4FB7-4FE2-8BDD-F4C1A7729277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Atalhos Intellij e STS</t>
   </si>
@@ -227,9 +227,6 @@
     <t>GitToolBox</t>
   </si>
   <si>
-    <t>Mostra os comentários dos ultimos commits</t>
-  </si>
-  <si>
     <t>Key Promoter X</t>
   </si>
   <si>
@@ -245,7 +242,195 @@
     <t>Translatiion</t>
   </si>
   <si>
-    <t>CTRL +SHIFT + O ==&gt; funciona como o google translation</t>
+    <t>Alt + Down/Up</t>
+  </si>
+  <si>
+    <t>desloca a linha verticalmente, sem a necessidade de copiar e colar.</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + down/up</t>
+  </si>
+  <si>
+    <t>Duplica a linha onde se encontra o cursor para cima ou para baixo sem precisar selecionar.</t>
+  </si>
+  <si>
+    <t>Alt + Shift + C</t>
+  </si>
+  <si>
+    <t>alterar a assinatura do método basta clicar em cima do mesmo e acionar o atalho. De forma simples e segura você conseguirá modificar coisas como o nome, visibilidade, tipo de retorno, parâmetros, etc.</t>
+  </si>
+  <si>
+    <t>Alt + Shift + A</t>
+  </si>
+  <si>
+    <t> é possível selecionar um bloco de código e modificar todas as linhas selecionadas simultaneamente. Para desativar basta precionar o atalho novamente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14996795556505021"/>
+        <rFont val="Lucida Sans"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CTRL +SHIFT + O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.14996795556505021"/>
+        <rFont val="Lucida Sans"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ==&gt; funciona como o google translation</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostra os comentários dos ultimos commits / Auto featch </t>
+  </si>
+  <si>
+    <t>one Dark Theme</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://plugins.jetbrains.com/plugin/11938-one-dark-theme</t>
+  </si>
+  <si>
+    <t>https://plugins.jetbrains.com/plugin/7499-gittoolbox</t>
+  </si>
+  <si>
+    <t>https://plugins.jetbrains.com/plugin/9792-key-promoter-x</t>
+  </si>
+  <si>
+    <t>https://plugins.jetbrains.com/plugin/8575-nyan-progress-bar</t>
+  </si>
+  <si>
+    <t>https://plugins.jetbrains.com/plugin/10080-rainbow-brackets</t>
+  </si>
+  <si>
+    <t>Nyan Progress Bar</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + X/Y</t>
+  </si>
+  <si>
+    <r>
+      <t>deixa a seleção maiúscula (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>) ou minúscula (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Ctrl + 3</t>
+  </si>
+  <si>
+    <r>
+      <t>Abre o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>Quick Access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t> onde é possível pesquisar pelas diversas funcionalidades do Eclipse. Eu uso para chamar o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>generate getters and setters, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>digitando apenas “gett”, e </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>generate constructor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF292929"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>, digitando apenas “const”.</t>
+    </r>
+  </si>
+  <si>
+    <t>Atom Material Icon</t>
+  </si>
+  <si>
+    <t>Mario Progress Bar</t>
   </si>
 </sst>
 </file>
@@ -259,7 +444,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -517,6 +702,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF292929"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF292929"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.14996795556505021"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF292929"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -705,7 +917,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -811,6 +1023,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC8F0FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
@@ -871,7 +1092,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -890,20 +1111,41 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -959,60 +1201,12 @@
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="13" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="20">
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFC8F0FF"/>
-        </bottom>
-      </border>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Rockwell"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFC8F0FF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Rockwell"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1020,12 +1214,6 @@
           <color theme="6" tint="0.79998168889431442"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1077,7 +1265,40 @@
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color theme="6" tint="0.79998168889431442"/>
+          <color rgb="FFC8F0FF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFC8F0FF"/>
         </bottom>
       </border>
     </dxf>
@@ -1181,14 +1402,14 @@
   </dxfs>
   <tableStyles count="2" defaultPivotStyle="PivotStyleLight18">
     <tableStyle name="Catálogo de endereços" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="secondRowStripe" dxfId="16"/>
     </tableStyle>
     <tableStyle name="Lista de tarefas pendentes" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1210,9 +1431,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5F05E028-106A-477F-9E02-C6C607BCF5B4}" name="ChavesDeCores6" displayName="ChavesDeCores6" ref="B3:B19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5F05E028-106A-477F-9E02-C6C607BCF5B4}" name="ChavesDeCores6" displayName="ChavesDeCores6" ref="B3:B19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B175FE8F-7974-47AD-946E-754F2B5A5B40}" name="PLUGIN" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B175FE8F-7974-47AD-946E-754F2B5A5B40}" name="PLUGIN" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Catálogo de endereços" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1224,9 +1445,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{834D91C4-FEA7-4EB6-A0FE-1F28E440ACED}" name="ChavesDeCores27" displayName="ChavesDeCores27" ref="C3:C19" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{834D91C4-FEA7-4EB6-A0FE-1F28E440ACED}" name="ChavesDeCores27" displayName="ChavesDeCores27" ref="C3:D19" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4E55BCA8-0E32-4712-BF7F-2ED8AB8D0AF2}" name="AÇÃO"/>
+    <tableColumn id="2" xr3:uid="{60FC4126-02C9-4EA4-A337-F9993C00B8C5}" name="Link"/>
   </tableColumns>
   <tableStyleInfo name="Catálogo de endereços" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1238,9 +1460,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ChavesDeCores" displayName="ChavesDeCores" ref="B3:B19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="9" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ChavesDeCores" displayName="ChavesDeCores" ref="B3:B25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="COMANDO " dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="COMANDO " dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Catálogo de endereços" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1252,9 +1474,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2C688A7-415A-4BB6-8AD8-D76F900682BD}" name="ChavesDeCores2" displayName="ChavesDeCores2" ref="C3:C19" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2C688A7-415A-4BB6-8AD8-D76F900682BD}" name="ChavesDeCores2" displayName="ChavesDeCores2" ref="C3:C25" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0" headerRowBorderDxfId="2">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{37FB3957-A2E6-461B-BFBB-8EB1C5083465}" name="AÇÃO"/>
+    <tableColumn id="1" xr3:uid="{37FB3957-A2E6-461B-BFBB-8EB1C5083465}" name="AÇÃO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Catálogo de endereços" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1498,8 +1720,8 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3278" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4275" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
@@ -1507,20 +1729,21 @@
     <col min="1" max="1" width="3.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="63.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.21875" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="15" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="10.77734375" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="66" customHeight="1">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1528,11 +1751,11 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="2:11" ht="83.25" customHeight="1">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1546,83 +1769,106 @@
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="30" customHeight="1">
+      <c r="B5" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1">
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="30" customHeight="1">
+      <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="30" customHeight="1">
+      <c r="B7" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1">
-      <c r="B6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1">
-      <c r="B7" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="30" customHeight="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:11" ht="30" customHeight="1">
-      <c r="B9" s="8"/>
+      <c r="B9" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="C9" s="2"/>
+      <c r="D9" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="2:11" ht="30" customHeight="1">
-      <c r="B10" s="8"/>
+      <c r="B10" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="2:11" ht="30" customHeight="1">
-      <c r="B11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="2:11" ht="30" customHeight="1">
-      <c r="B12" s="8"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="2:11" ht="30" customHeight="1">
-      <c r="B13" s="8"/>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="2:11" ht="30" customHeight="1">
-      <c r="B14" s="8"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1">
-      <c r="B15" s="8"/>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" spans="2:11" ht="30" customHeight="1">
-      <c r="B16" s="8"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="2:2" ht="30" customHeight="1">
-      <c r="B17" s="9"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="2:2" ht="30" customHeight="1">
-      <c r="B18" s="9"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="2:2" ht="30" customHeight="1">
-      <c r="B19" s="9"/>
+      <c r="B19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1654,17 +1900,17 @@
     <tabColor theme="6" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.21875" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="15" width="0" style="1" hidden="1" customWidth="1"/>
@@ -1672,13 +1918,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="66" customHeight="1">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1686,11 +1932,11 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="2:11" ht="83.25" customHeight="1">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1711,132 +1957,180 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" customHeight="1">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="30" customHeight="1">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="30" customHeight="1">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:11" ht="30" customHeight="1">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" customHeight="1">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" customHeight="1">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="30" customHeight="1">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="30" customHeight="1">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="30" customHeight="1">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="30" customHeight="1">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="30" customHeight="1">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" customHeight="1">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" customHeight="1">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="16" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="30" customHeight="1">
+      <c r="B20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="30" customHeight="1">
+      <c r="B21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="42" customHeight="1">
+      <c r="B22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="30" customHeight="1">
+      <c r="B23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="30" customHeight="1">
+      <c r="B24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="65.25" customHeight="1">
+      <c r="B25" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1864,12 +2158,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2081,20 +2375,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2120,9 +2412,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>